<commit_message>
Bill Avocado day 6
</commit_message>
<xml_diff>
--- a/data/B/experiment4/avocadEx4.xlsx
+++ b/data/B/experiment4/avocadEx4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koohong\Documents\MIDS\MIDS241\mids-w241-fa2020-fp\data\B\experiment4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B635C072-8326-4B1F-9F24-5B240B84A97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3776063-A6F6-4974-AF81-E32B3A50A22D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M13"/>
+      <selection activeCell="N2" sqref="N2:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +517,12 @@
       <c r="M2">
         <v>73</v>
       </c>
+      <c r="N2">
+        <v>45</v>
+      </c>
+      <c r="O2">
+        <v>72</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -558,6 +564,12 @@
       <c r="M3">
         <v>73</v>
       </c>
+      <c r="N3">
+        <v>45</v>
+      </c>
+      <c r="O3">
+        <v>72</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -599,6 +611,12 @@
       <c r="M4">
         <v>73</v>
       </c>
+      <c r="N4">
+        <v>45</v>
+      </c>
+      <c r="O4">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -640,6 +658,12 @@
       <c r="M5">
         <v>73</v>
       </c>
+      <c r="N5">
+        <v>45</v>
+      </c>
+      <c r="O5">
+        <v>72</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -681,6 +705,12 @@
       <c r="M6">
         <v>73</v>
       </c>
+      <c r="N6">
+        <v>45</v>
+      </c>
+      <c r="O6">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -722,6 +752,12 @@
       <c r="M7">
         <v>73</v>
       </c>
+      <c r="N7">
+        <v>45</v>
+      </c>
+      <c r="O7">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -763,6 +799,12 @@
       <c r="M8">
         <v>73</v>
       </c>
+      <c r="N8">
+        <v>45</v>
+      </c>
+      <c r="O8">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -804,6 +846,12 @@
       <c r="M9">
         <v>73</v>
       </c>
+      <c r="N9">
+        <v>45</v>
+      </c>
+      <c r="O9">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -845,6 +893,12 @@
       <c r="M10">
         <v>73</v>
       </c>
+      <c r="N10">
+        <v>45</v>
+      </c>
+      <c r="O10">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -886,6 +940,12 @@
       <c r="M11">
         <v>73</v>
       </c>
+      <c r="N11">
+        <v>45</v>
+      </c>
+      <c r="O11">
+        <v>72</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -927,6 +987,12 @@
       <c r="M12">
         <v>73</v>
       </c>
+      <c r="N12">
+        <v>45</v>
+      </c>
+      <c r="O12">
+        <v>72</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -967,6 +1033,12 @@
       </c>
       <c r="M13">
         <v>73</v>
+      </c>
+      <c r="N13">
+        <v>45</v>
+      </c>
+      <c r="O13">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>